<commit_message>
Update Conditional Formatting Excel Tutorial File.xlsx
</commit_message>
<xml_diff>
--- a/Excel/Lesson_23/Conditional Formatting Excel Tutorial File.xlsx
+++ b/Excel/Lesson_23/Conditional Formatting Excel Tutorial File.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\.vscode\Data_Analyst_Bootcamp\Data_Analyst_Bootcamp\Excel\Lesson_23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE12AABD-2C2A-4D60-B298-E861FD33474F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
     <sheet name="Sales" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Demographics!$A$1:$K$23</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -290,12 +292,18 @@
   </si>
   <si>
     <t>Manila Folder</t>
+  </si>
+  <si>
+    <t>Can filter and sort by color</t>
+  </si>
+  <si>
+    <t>Careful of autofill to apply color on all cells</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -333,7 +341,208 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -642,29 +851,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1027015F-D30F-450C-928C-DE78480974B7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -699,7 +908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -734,7 +943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -769,7 +978,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -804,7 +1013,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -839,7 +1048,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -874,7 +1083,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -909,7 +1118,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -944,7 +1153,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -979,7 +1188,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1014,37 +1223,74 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" t="str">
-        <f t="shared" ref="D22:D23" si="0">CONCATENATE(B12," ",C12)</f>
+        <f>CONCATENATE(B12," ",C12)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(B13," ",C13)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="iconSet" priority="11">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G10">
+    <cfRule type="duplicateValues" dxfId="13" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>$H$2&gt; 50000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>H3&gt;50000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>H4&gt;50000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CCAA7F-6F85-4102-B7D4-D80770622F9F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B4" sqref="B4:M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>72</v>
       </c>
@@ -1082,7 +1328,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1123,7 +1369,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1164,7 +1410,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -1206,6 +1452,42 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:M2">
+    <cfRule type="iconSet" priority="4">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:M3">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:M4">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="5Arrows">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="20"/>
+        <cfvo type="percent" val="40"/>
+        <cfvo type="percent" val="60"/>
+        <cfvo type="percent" val="80"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>